<commit_message>
Testing the models with one variable
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -76,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,23 +161,22 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="17.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -222,10 +222,76 @@
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="0" t="n">
+        <v>0.647619047619048</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.679365079365079</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.683333333333333</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.651587301587302</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.678571428571429</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.647619047619048</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0.653968253968254</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.664285714285714</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0.662698412698413</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.672222222222222</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.664285714285714</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.662698412698413</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0.673015873015873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting P-values from linear regression
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Model/Feature</t>
   </si>
@@ -62,14 +62,27 @@
   </si>
   <si>
     <t xml:space="preserve">Logistic regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valores muy cercanos a cero indican alta relacion entre X e Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tambien indican que es muy poco probable encontrar relacion entre X e Y por azar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -94,12 +107,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,8 +155,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,6 +185,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -158,23 +253,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L2:L4"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="17.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
@@ -187,10 +282,10 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -199,7 +294,7 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
@@ -214,7 +309,7 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -225,10 +320,10 @@
       <c r="B2" s="0" t="n">
         <v>0.647619047619048</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.679365079365079</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.683333333333333</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -237,7 +332,7 @@
       <c r="F2" s="0" t="n">
         <v>0.651587301587302</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0.678571428571429</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -252,7 +347,7 @@
       <c r="K2" s="0" t="n">
         <v>0.664285714285714</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.662698412698413</v>
       </c>
     </row>
@@ -263,10 +358,10 @@
       <c r="B3" s="0" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.672222222222222</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.665873015873016</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -275,7 +370,7 @@
       <c r="F3" s="0" t="n">
         <v>0.662698412698413</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>0.665873015873016</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -290,8 +385,61 @@
       <c r="K3" s="0" t="n">
         <v>0.665873015873016</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>0.673015873015873</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.470242504</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.0558321578</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.988234525</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>1.24599779E-084</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0.908072679</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>2.96703179E-181</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>0.999999999</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>0.999119348</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0.997358586</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>4.98285632E-025</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Printing graphs and analizing them
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">One variable</t>
+  </si>
   <si>
     <t xml:space="preserve">Model/Feature</t>
   </si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Logistic regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two variables</t>
   </si>
   <si>
     <t xml:space="preserve">Linear regression</t>
@@ -155,16 +161,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,10 +255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -279,167 +281,212 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J2" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K2" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L2" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.647619047619048</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.679365079365079</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.683333333333333</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0.651587301587302</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>0.678571428571429</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0.647619047619048</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0.653968253968254</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>0.664285714285714</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>0.662698412698413</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
+        <v>0.647619047619048</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.679365079365079</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.683333333333333</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="F4" s="0" t="n">
+        <v>0.651587301587302</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.678571428571429</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.647619047619048</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.653968253968254</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.664285714285714</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0.662698412698413</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>0.672222222222222</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="D5" s="1" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>0.664285714285714</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>0.662698412698413</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>0.665873015873016</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="G5" s="1" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.665873015873016</v>
+      </c>
+      <c r="L5" s="1" t="n">
         <v>0.673015873015873</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="n">
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2" t="n">
         <v>0.470242504</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C28" s="2" t="n">
         <v>0.0558321578</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D28" s="2" t="n">
         <v>0.988234525</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E28" s="3" t="n">
         <v>1.24599779E-084</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F28" s="2" t="n">
         <v>0.908072679</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G28" s="3" t="n">
         <v>2.96703179E-181</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H28" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I28" s="2" t="n">
         <v>0.999999999</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J28" s="2" t="n">
         <v>0.999119348</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="K28" s="2" t="n">
         <v>0.997358586</v>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L28" s="3" t="n">
         <v>4.98285632E-025</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>17</v>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>